<commit_message>
Update gitignore and Stock Table
</commit_message>
<xml_diff>
--- a/Stock Table.xlsx
+++ b/Stock Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QuantML\VS_QuantMLV6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF3B8D7-4CDF-408A-8AC5-965AE63BA750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E428BDDF-0A60-4761-A7AC-FB16B9F11212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,10 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -95,6 +91,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>130080</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114518</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F245089C-91A3-DD25-7AA5-1369A81CFFBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6226080" cy="2514818"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -362,9 +407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -373,5 +416,6 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>